<commit_message>
El AI Engine usa los datos en la carpeta en linea
</commit_message>
<xml_diff>
--- a/AI_Engine/Resultados/EMP/dataFrame.xlsx
+++ b/AI_Engine/Resultados/EMP/dataFrame.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:G1"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,812 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>R136513</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Prior</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>R136513</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>448.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>08/01/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>R136513</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>448.0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>12/05/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>R136513</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>448.0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>06/05/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>9,781.0</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>PAST DUE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3,932.0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>06/06/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4,915.0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>07/01/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>5,898.0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>09/02/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>4,915.0</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>10/03/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>4,915.0</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>11/07/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>5,898.0</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>12/05/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>4,915.0</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>12/28/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>3,932.0</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>02/06/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>4,915.0</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>03/06/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>4,915.0</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>05/01/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>4,915.0</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>06/05/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>4,915.0</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>07/03/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3,932.0</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>08/07/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>R519291</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1,966.0</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>10/02/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>R521456</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Prior</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>R521456</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>06/06/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>R521456</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1,655.0</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>08/29/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>R521456</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>1,655.0</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>11/07/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>R521456</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1,655.0</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>12/05/22</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>R521456</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1,655.0</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>05/01/23</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>C:\Users\IRDGFRM\Downloads\MR00210221_220505043902_67.pdf</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>G0210221</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>R521456</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1,655.0</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>07/03/23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>